<commit_message>
Short document and page comments
</commit_message>
<xml_diff>
--- a/data_analyzed/regression.xlsx
+++ b/data_analyzed/regression.xlsx
@@ -441,22 +441,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Beta_M1_PH</t>
+          <t>Beta_M1_RN</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Beta_CM2_PH</t>
+          <t>Beta_CM2_RN</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Beta_CMN3_PH</t>
+          <t>Beta_CMN3_RN</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Beta_CMN4_PH</t>
+          <t>Beta_CMN4_RN</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Updating processed and analyzed data. Need to take incremental from next time.
</commit_message>
<xml_diff>
--- a/data_analyzed/regression.xlsx
+++ b/data_analyzed/regression.xlsx
@@ -477,10 +477,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.528728191020881</v>
+        <v>1.255084099591062</v>
       </c>
       <c r="C2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>-0</v>
@@ -489,10 +489,10 @@
         <v>-0</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.005501763637493055</v>
+        <v>-0.07526281778284652</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1121107236151534</v>
+        <v>0.06112493876441671</v>
       </c>
     </row>
     <row r="3">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-8.856209988319669e-17</v>
+        <v>-0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -514,7 +514,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.09480635032960948</v>
+        <v>0.1146013691737822</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -539,7 +539,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.1954126268272056</v>
+        <v>-0.1651586729926508</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -552,22 +552,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.11426957424362</v>
+        <v>1.070040597132289e-15</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1518058952079546</v>
+        <v>-0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02603950807985474</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>-0</v>
       </c>
       <c r="F5" t="n">
-        <v>2.438082653878514</v>
+        <v>2.343275768088881</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01599668415018052</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removing less than USD 5 price from extrapolation calibration because it is just a noise
</commit_message>
<xml_diff>
--- a/data_analyzed/regression.xlsx
+++ b/data_analyzed/regression.xlsx
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.107732738556743</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -486,13 +486,13 @@
         <v>-0</v>
       </c>
       <c r="E2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.07685546929357041</v>
+        <v>-0.06579314222947109</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0489949390430966</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -502,22 +502,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0</v>
+        <v>-0.07909600764659845</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.9807047427925161</v>
       </c>
       <c r="D3" t="n">
-        <v>-0</v>
+        <v>0.01265768756098197</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.007990346254841385</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1122065998459664</v>
+        <v>-0.1018343811709898</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.1673002035305011</v>
       </c>
     </row>
     <row r="4">
@@ -527,22 +527,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="C4" t="n">
-        <v>-0</v>
+        <v>-6.404326871522143</v>
       </c>
       <c r="D4" t="n">
-        <v>-0</v>
+        <v>-0.2425370427083099</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>-0.02784059730917719</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.1274192750328835</v>
+        <v>0.9193718120583519</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.1298556790611475</v>
       </c>
     </row>
     <row r="5">
@@ -552,22 +552,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>9.988614479079335e-16</v>
+        <v>1.165621356363873</v>
       </c>
       <c r="C5" t="n">
-        <v>-0</v>
+        <v>5.022181165303445</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.4156892904508752</v>
       </c>
       <c r="E5" t="n">
-        <v>-0</v>
+        <v>0.04685879615052199</v>
       </c>
       <c r="F5" t="n">
-        <v>2.307198741644828</v>
+        <v>1.423691301974722</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.06494495314546911</v>
       </c>
     </row>
   </sheetData>

</xml_diff>